<commit_message>
update to new excel format
</commit_message>
<xml_diff>
--- a/Hoe-ben-je-bij-mij-terecht-gekomen.xlsx
+++ b/Hoe-ben-je-bij-mij-terecht-gekomen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b5c70f5e09435a15/Bureaublad/E-doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\Mimosa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{1741BF52-09E2-4E5C-8956-4F6D8E3FCC7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{47602526-7FEB-452B-8678-B8E9AAAE67A6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26123294-27CD-4429-AE54-A3C9A1BD35E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{60AEE2C5-860D-487A-9BAE-A2D08552E2E5}"/>
+    <workbookView xWindow="3045" yWindow="2505" windowWidth="21600" windowHeight="11385" xr2:uid="{60AEE2C5-860D-487A-9BAE-A2D08552E2E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Hoe ben je bij mij terecht gekomen?</t>
   </si>
@@ -40,9 +42,6 @@
   </si>
   <si>
     <t>Website</t>
-  </si>
-  <si>
-    <t>Krantje</t>
   </si>
   <si>
     <t>Logopedie</t>
@@ -54,7 +53,19 @@
     <t>Anders</t>
   </si>
   <si>
-    <t>Doorverwijzing psycholoog</t>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Psycholoog</t>
+  </si>
+  <si>
+    <t>Onbekend</t>
+  </si>
+  <si>
+    <t>Update:</t>
+  </si>
+  <si>
+    <t>Krantje</t>
   </si>
 </sst>
 </file>
@@ -90,11 +101,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -112,7 +125,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -149,7 +162,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="nl-BE"/>
+              <a:rPr lang="en-US"/>
               <a:t>Hoe ben je bij mij terecht gekomen?</a:t>
             </a:r>
           </a:p>
@@ -186,7 +199,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="LID4096"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -200,6 +213,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Huisarts</c:v>
+          </c:tx>
           <c:spPr>
             <a:gradFill rotWithShape="1">
               <a:gsLst>
@@ -239,60 +255,202 @@
             </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Blad1!$B$3:$B$9</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Huisarts</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Website</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Krantje</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Logopedie</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Kennis</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Anders</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Doorverwijzing psycholoog</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$C$3:$C$9</c:f>
+              <c:f>Blad1!$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2714-4C28-B3B1-5FD091D0AC01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Website</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="2">
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2714-4C28-B3B1-5FD091D0AC01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Krantje</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2714-4C28-B3B1-5FD091D0AC01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Kennis</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -300,7 +458,265 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-99D7-479F-B594-64BCB9E1EEA7}"/>
+              <c16:uniqueId val="{00000003-2714-4C28-B3B1-5FD091D0AC01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Psycholoog</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-2714-4C28-B3B1-5FD091D0AC01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Logopedie</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-2714-4C28-B3B1-5FD091D0AC01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Ander</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-2714-4C28-B3B1-5FD091D0AC01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>Onbekend</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$I$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-2714-4C28-B3B1-5FD091D0AC01}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -312,25 +728,31 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="189638815"/>
-        <c:axId val="249208495"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="1355707327"/>
+        <c:axId val="1355708991"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="189638815"/>
+        <c:axId val="1355707327"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -350,10 +772,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="LID4096"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249208495"/>
+        <c:crossAx val="1355708991"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -361,7 +783,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="249208495"/>
+        <c:axId val="1355708991"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -371,9 +793,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -408,10 +830,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="LID4096"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189638815"/>
+        <c:crossAx val="1355707327"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -423,6 +845,36 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -467,13 +919,13 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="LID4096"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+    <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -519,7 +971,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="294">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -540,7 +992,17 @@
         <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr/>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea>
@@ -612,7 +1074,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -622,7 +1084,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -632,7 +1094,7 @@
     <cs:fillRef idx="3"/>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="34925" cap="rnd">
@@ -652,7 +1114,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -671,7 +1133,7 @@
     <cs:fillRef idx="3"/>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -708,7 +1170,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -732,7 +1194,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -751,7 +1213,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -769,7 +1231,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -777,14 +1239,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -796,14 +1258,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -814,7 +1276,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -833,7 +1295,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -862,7 +1324,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -870,7 +1332,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -882,7 +1344,17 @@
         <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr/>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -930,7 +1402,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
@@ -956,7 +1428,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -988,7 +1460,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -998,23 +1470,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Grafiek 2">
+        <xdr:cNvPr id="2" name="Grafiek 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDB369BB-6C69-41A6-A50F-910C71AEF6FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1E390CF-F965-4D75-8836-8F0F950176F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1035,8 +1507,26 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1191EA1-1F82-433B-9D5B-D541EBA61099}" name="Tabel1" displayName="Tabel1" ref="A4:I55" totalsRowCount="1">
+  <autoFilter ref="A4:I54" xr:uid="{85BAA4E9-2CB8-4E28-86E6-1A8D65B3F1E1}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{B78E103F-F07C-4FD8-9237-C45D04850FF3}" name="#"/>
+    <tableColumn id="2" xr3:uid="{D9583DDC-AF31-4256-9277-74700BEC7131}" name="Huisarts"/>
+    <tableColumn id="3" xr3:uid="{0A7629FB-C33F-407A-852F-D85AF2C40506}" name="Website"/>
+    <tableColumn id="4" xr3:uid="{4832AB3D-8739-42CE-8A88-484644D3D455}" name="Krantje"/>
+    <tableColumn id="5" xr3:uid="{EF478603-ED8D-4446-A5B5-EF44B2BD02CE}" name="Kennis"/>
+    <tableColumn id="6" xr3:uid="{B6457FEF-CB69-49AE-9F9C-56F26847AD4E}" name="Psycholoog"/>
+    <tableColumn id="7" xr3:uid="{57AD24F2-C99D-4FB8-80F6-A025B9F13414}" name="Logopedie"/>
+    <tableColumn id="8" xr3:uid="{F66BDC5F-C4D0-4EC9-8C98-B43D1C1AFE6B}" name="Anders"/>
+    <tableColumn id="9" xr3:uid="{3BFB7904-6643-4FB5-95D3-4C16B02196FE}" name="Onbekend"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1332,77 +1822,448 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F1B368-E893-4CFD-865B-B5B27D341DB2}">
-  <dimension ref="A2:C9"/>
+  <dimension ref="A2:L54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>1</v>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f>SUM(Tabel1[Huisarts])</f>
+        <v>5</v>
       </c>
       <c r="C3">
+        <f>SUM(Tabel1[Website])</f>
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <f>SUM(Tabel1[Krantje])</f>
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <f>SUM(Tabel1[Kennis])</f>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f>SUM(Tabel1[Psycholoog])</f>
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <f>SUM(Tabel1[Logopedie])</f>
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <f>SUM(Tabel1[Anders])</f>
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <f>SUM(Tabel1[Onbekend])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>6</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>7</v>
       </c>
-      <c r="C9">
-        <v>1</v>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="K24" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" s="1">
+        <v>44284</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>28</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>